<commit_message>
Switches - front panel - wip
</commit_message>
<xml_diff>
--- a/modules/Switches/panel/positions.xlsx
+++ b/modules/Switches/panel/positions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\Switches\panel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Switches\panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCE4B3F-12B7-4EB1-B592-DF72A86F79D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC86C66-4239-401D-A81F-524068DF442B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{570610C3-5DB8-4413-A76C-348D2E1B3E85}"/>
+    <workbookView xWindow="6705" yWindow="1500" windowWidth="18540" windowHeight="12495" xr2:uid="{570610C3-5DB8-4413-A76C-348D2E1B3E85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>PCB x</t>
   </si>
@@ -63,6 +63,39 @@
   </si>
   <si>
     <t>height offset</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>SW4</t>
   </si>
 </sst>
 </file>
@@ -414,15 +447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AEE469-D859-4D2F-91A1-64B02B71ECC5}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -453,7 +486,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -464,7 +497,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -477,7 +510,7 @@
         <v>23.32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -490,7 +523,7 @@
         <v>29.817999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -503,9 +536,9 @@
         <v>25.82</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>105.9</v>
@@ -520,6 +553,182 @@
       <c r="E7">
         <f>C7+$C$5</f>
         <v>68.201999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>115.61750000000001</v>
+      </c>
+      <c r="C8">
+        <v>38.384</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D14" si="0">B8+$B$5</f>
+        <v>75.1875</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E14" si="1">C8+$C$5</f>
+        <v>68.201999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>105.9</v>
+      </c>
+      <c r="C9">
+        <v>69.700666999999996</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>65.47</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>99.518666999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-40.430000000000007</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>29.817999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>101.01733299999999</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-40.430000000000007</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>130.83533299999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-40.430000000000007</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>29.817999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>132.334</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-40.430000000000007</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>162.15199999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-40.430000000000007</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>29.817999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>131.97999999999999</v>
+      </c>
+      <c r="C15">
+        <v>42.457999999999998</v>
+      </c>
+      <c r="D15">
+        <f>B15+$B$6</f>
+        <v>94.049999999999983</v>
+      </c>
+      <c r="E15">
+        <f>C15+$C$6</f>
+        <v>68.277999999999992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>73.774666999999994</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D18" si="2">B16+$B$6</f>
+        <v>-37.930000000000007</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E18" si="3">C16+$C$6</f>
+        <v>99.594666999999987</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>105.09133300000001</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>-37.930000000000007</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>130.91133300000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>136.40799999999999</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>-37.930000000000007</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>162.22799999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switches - panel graphics
</commit_message>
<xml_diff>
--- a/modules/Switches/panel/positions.xlsx
+++ b/modules/Switches/panel/positions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Switches\panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC86C66-4239-401D-A81F-524068DF442B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C018A2D2-1022-4777-A95D-FB4C827FC013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="1500" windowWidth="18540" windowHeight="12495" xr2:uid="{570610C3-5DB8-4413-A76C-348D2E1B3E85}"/>
+    <workbookView xWindow="405" yWindow="1335" windowWidth="18540" windowHeight="12495" xr2:uid="{570610C3-5DB8-4413-A76C-348D2E1B3E85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>PCB x</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>SW4</t>
+  </si>
+  <si>
+    <t>svg x</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>arrow tops</t>
+  </si>
+  <si>
+    <t>lines top</t>
   </si>
 </sst>
 </file>
@@ -447,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AEE469-D859-4D2F-91A1-64B02B71ECC5}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +480,23 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -486,7 +513,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -497,7 +524,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -510,7 +537,7 @@
         <v>23.32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -523,7 +550,7 @@
         <v>29.817999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -535,8 +562,12 @@
         <f>2.5+C4</f>
         <v>25.82</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f>E9-E8</f>
+        <v>31.316666999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -554,8 +585,39 @@
         <f>C7+$C$5</f>
         <v>68.201999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>6.3</v>
+      </c>
+      <c r="G7">
+        <f>D7-$F$7/2</f>
+        <v>62.32</v>
+      </c>
+      <c r="H7">
+        <f>E7-$F$7/2</f>
+        <v>65.051999999999992</v>
+      </c>
+      <c r="I7">
+        <v>73.394000000000005</v>
+      </c>
+      <c r="J7">
+        <f>I7-H7</f>
+        <v>8.342000000000013</v>
+      </c>
+      <c r="K7">
+        <v>67.287999999999997</v>
+      </c>
+      <c r="L7">
+        <f>K7-H7</f>
+        <v>2.2360000000000042</v>
+      </c>
+      <c r="M7">
+        <v>72.180999999999997</v>
+      </c>
+      <c r="N7">
+        <v>66.147999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -573,8 +635,16 @@
         <f t="shared" ref="E8:E14" si="1">C8+$C$5</f>
         <v>68.201999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" ref="G8:G15" si="2">D8-$F$7/2</f>
+        <v>72.037499999999994</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:H14" si="3">E8-$F$7/2</f>
+        <v>65.051999999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -592,79 +662,195 @@
         <f t="shared" si="1"/>
         <v>99.518666999999994</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>62.32</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>96.368666999999988</v>
+      </c>
+      <c r="I9">
+        <f>H9+$J$7</f>
+        <v>104.710667</v>
+      </c>
+      <c r="K9">
+        <f>H9+$L$7</f>
+        <v>98.604666999999992</v>
+      </c>
+      <c r="M9">
+        <f>M7+$M$6</f>
+        <v>103.49766699999999</v>
+      </c>
+      <c r="N9">
+        <f>N7+$M$6</f>
+        <v>97.464666999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="B10">
+        <v>115.61750000000001</v>
+      </c>
+      <c r="C10">
+        <v>69.700666999999996</v>
+      </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>-40.430000000000007</v>
+        <v>75.1875</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>29.817999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99.518666999999994</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>72.037499999999994</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>96.368666999999988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="B11">
+        <v>105.9</v>
+      </c>
       <c r="C11">
         <v>101.01733299999999</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>-40.430000000000007</v>
+        <v>65.47</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
         <v>130.83533299999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>62.32</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>127.68533299999999</v>
+      </c>
+      <c r="I11">
+        <f>H11+$J$7</f>
+        <v>136.027333</v>
+      </c>
+      <c r="K11">
+        <f>H11+$L$7</f>
+        <v>129.921333</v>
+      </c>
+      <c r="M11">
+        <f>M9+$M$6</f>
+        <v>134.81433399999997</v>
+      </c>
+      <c r="N11">
+        <f>N9+$M$6</f>
+        <v>128.78133399999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12">
+        <v>115.61750000000001</v>
+      </c>
+      <c r="C12">
+        <v>101.01733299999999</v>
+      </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-40.430000000000007</v>
+        <v>75.1875</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>29.817999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>130.83533299999999</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>72.037499999999994</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>127.68533299999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
+      <c r="B13">
+        <v>105.9</v>
+      </c>
       <c r="C13">
         <v>132.334</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>-40.430000000000007</v>
+        <v>65.47</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
         <v>162.15199999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>62.32</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>159.00199999999998</v>
+      </c>
+      <c r="I13">
+        <f>H13+$J$7</f>
+        <v>167.34399999999999</v>
+      </c>
+      <c r="K13">
+        <f>H13+$L$7</f>
+        <v>161.238</v>
+      </c>
+      <c r="N13">
+        <f>N11+$M$6</f>
+        <v>160.09800099999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="B14">
+        <v>115.61750000000001</v>
+      </c>
+      <c r="C14">
+        <v>132.334</v>
+      </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-40.430000000000007</v>
+        <v>75.1875</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>29.817999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>162.15199999999999</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>72.037499999999994</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>159.00199999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -682,53 +868,97 @@
         <f>C15+$C$6</f>
         <v>68.277999999999992</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>9.5</v>
+      </c>
+      <c r="G15">
+        <f>D15-$F$15/2</f>
+        <v>89.299999999999983</v>
+      </c>
+      <c r="H15">
+        <f>E15-$F$15/2</f>
+        <v>63.527999999999992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
+      <c r="B16">
+        <v>131.97999999999999</v>
+      </c>
       <c r="C16">
         <v>73.774666999999994</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:D18" si="2">B16+$B$6</f>
-        <v>-37.930000000000007</v>
+        <f t="shared" ref="D16:D18" si="4">B16+$B$6</f>
+        <v>94.049999999999983</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16:E18" si="3">C16+$C$6</f>
+        <f t="shared" ref="E16:E18" si="5">C16+$C$6</f>
         <v>99.594666999999987</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" ref="G16:G18" si="6">D16-$F$15/2</f>
+        <v>89.299999999999983</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H18" si="7">E16-$F$15/2</f>
+        <v>94.844666999999987</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
+      <c r="B17">
+        <v>131.97999999999999</v>
+      </c>
       <c r="C17">
         <v>105.09133300000001</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
-        <v>-37.930000000000007</v>
+        <f t="shared" si="4"/>
+        <v>94.049999999999983</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>130.91133300000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="6"/>
+        <v>89.299999999999983</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="7"/>
+        <v>126.16133300000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
+      <c r="B18">
+        <v>131.97999999999999</v>
+      </c>
       <c r="C18">
         <v>136.40799999999999</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
-        <v>-37.930000000000007</v>
+        <f t="shared" si="4"/>
+        <v>94.049999999999983</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>162.22799999999998</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="6"/>
+        <v>89.299999999999983</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="7"/>
+        <v>157.47799999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>